<commit_message>
Added clinic system agent description and appointment system agent description, updated role schema and interaction model
</commit_message>
<xml_diff>
--- a/GroupD_RolesModel+InteractionModels.xlsx
+++ b/GroupD_RolesModel+InteractionModels.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/anish_mukherjee1_ucalgary_ca/Documents/Desktop/SENG 696/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8006a4da2089a8b4/Desktop/SENG 696- Agent Based Engg/SENG696_GroupD/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_AA6956E1F55F1236E0DDEC72661B633518F0C76C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FDA283D-4D42-442C-82D3-EB6F49FFF4A0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Role Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="Interaction Model" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Role Schema</t>
   </si>
@@ -140,12 +141,63 @@
   </si>
   <si>
     <t>The service will listen to the appointment agent for a trigger. Once received, it will invoke the respective API to provide a meeting link to the user. Also, it will send a mail to the doctor to provide the patient feedback.</t>
+  </si>
+  <si>
+    <t>searchProfile</t>
+  </si>
+  <si>
+    <t>Search in Database for user profile</t>
+  </si>
+  <si>
+    <t>SearchDatabase</t>
+  </si>
+  <si>
+    <t>read Userprofile, write Database</t>
+  </si>
+  <si>
+    <t>newProfile = SearchDatabase.service</t>
+  </si>
+  <si>
+    <t>Successfully creating a profile</t>
+  </si>
+  <si>
+    <t>createAppointment</t>
+  </si>
+  <si>
+    <t>Creating new and successful appointment</t>
+  </si>
+  <si>
+    <t>createAppointment = createApppointment.service</t>
+  </si>
+  <si>
+    <t>Successfully generating an Appointment</t>
+  </si>
+  <si>
+    <t>searchDatabase</t>
+  </si>
+  <si>
+    <t>To search in databases for any user profile already exists</t>
+  </si>
+  <si>
+    <t>Clinic system</t>
+  </si>
+  <si>
+    <t>searchDatabse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If any registered user visits portal, it will search the database for its previous logs and details and share it with the physician. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a new and repeated appointments with the doctor for the users  </t>
+  </si>
+  <si>
+    <t>When a user wish to consult a physician, this service will generate appointments for the user with the physician. It will store the appointments in the database so that reminders can be sent.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,18 +446,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -415,7 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -438,6 +477,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,199 +777,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="F3:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="63.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="4" t="s">
+    <row r="3" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="7"/>
+      <c r="H8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="21"/>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="7"/>
+      <c r="H16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="21"/>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="7"/>
+      <c r="H24" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="21"/>
       <c r="G25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="21"/>
+      <c r="G33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="19"/>
+      <c r="H36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="19"/>
+      <c r="H37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="19"/>
+      <c r="H38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="H39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="21"/>
+      <c r="G41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:F25"/>
+  <mergeCells count="25">
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
@@ -926,6 +1089,21 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -933,101 +1111,121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D4:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="14" t="s">
+    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="4:9" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="15" t="s">
+    <row r="6" spans="4:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="17" t="s">
+      <c r="E6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="15" t="s">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="15" t="s">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="4:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="22" t="s">
+    <row r="9" spans="4:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16" t="s">
+      <c r="E9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1038,15 +1236,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100167A42814A0A7A429FBAAD58A3662C43" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e0f0b35447dfaef00fa2716150d7de8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8" xmlns:ns4="ce8d2f3a-208b-4f58-bb79-4192d7cf8650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b4fe6bd1d6509f7a3dbc01590a646f" ns3:_="" ns4:_="">
     <xsd:import namespace="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
@@ -1275,6 +1464,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1282,14 +1480,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E9EDBE-6CCD-4A05-942D-0FB6EAB02CCA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1304,6 +1494,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added Changes for Assignment #2 Signed-off-by: anish30145784 <anish.mukherjee1@ucalgary.ca>
</commit_message>
<xml_diff>
--- a/GroupD_RolesModel+InteractionModels.xlsx
+++ b/GroupD_RolesModel+InteractionModels.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8006a4da2089a8b4/Desktop/SENG 696- Agent Based Engg/SENG696_GroupD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\GroupD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_AA6956E1F55F1236E0DDEC72661B633518F0C76C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FDA283D-4D42-442C-82D3-EB6F49FFF4A0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Role Schema" sheetId="1" r:id="rId1"/>
     <sheet name="Interaction Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Exceptions_ClientAgent" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>Role Schema</t>
   </si>
@@ -192,12 +192,60 @@
   </si>
   <si>
     <t>When a user wish to consult a physician, this service will generate appointments for the user with the physician. It will store the appointments in the database so that reminders can be sent.</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>System Not Accessible at this point</t>
+  </si>
+  <si>
+    <t>Error Message is generated stating that stystem is not accessible.</t>
+  </si>
+  <si>
+    <t>Relationships:</t>
+  </si>
+  <si>
+    <t>Initiating</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Collaborating</t>
+  </si>
+  <si>
+    <t>Notification Agent, Appointment Agent</t>
+  </si>
+  <si>
+    <t>Other Diagrams:</t>
+  </si>
+  <si>
+    <t>Data Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Required : </t>
+  </si>
+  <si>
+    <t>Data Required for Appointment Agent</t>
+  </si>
+  <si>
+    <t>Pet Information</t>
+  </si>
+  <si>
+    <t>Appointment Preferences</t>
+  </si>
+  <si>
+    <t>Client Information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +276,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -433,11 +487,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -478,6 +603,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,8 +618,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,60 +951,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="63.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="18" t="s">
+    <row r="3" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="18" t="s">
+    <row r="5" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="18" t="s">
+    <row r="6" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="18" t="s">
+    <row r="7" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="20" t="s">
+    <row r="8" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -840,8 +1014,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="21"/>
+    <row r="9" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="22"/>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
@@ -849,45 +1023,45 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="18" t="s">
+    <row r="11" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="18" t="s">
+    <row r="13" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F13" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="18" t="s">
+    <row r="14" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="18" t="s">
+    <row r="15" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="20" t="s">
+    <row r="16" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -897,8 +1071,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="21"/>
+    <row r="17" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="22"/>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
@@ -906,45 +1080,45 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="18" t="s">
+    <row r="19" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="18" t="s">
+    <row r="21" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="18" t="s">
+    <row r="22" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="18" t="s">
+    <row r="23" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="20" t="s">
+    <row r="24" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -954,8 +1128,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="21"/>
+    <row r="25" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="22"/>
       <c r="G25" s="3" t="s">
         <v>6</v>
       </c>
@@ -963,45 +1137,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="18" t="s">
+    <row r="27" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="18" t="s">
+    <row r="29" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="18" t="s">
+    <row r="30" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="18" t="s">
+    <row r="31" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F31" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="20" t="s">
+    <row r="32" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="5" t="s">
@@ -1011,8 +1185,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="21"/>
+    <row r="33" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="22"/>
       <c r="G33" s="3" t="s">
         <v>6</v>
       </c>
@@ -1020,45 +1194,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="18" t="s">
+    <row r="35" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F36" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="18" t="s">
+    <row r="37" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F37" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F38" s="18" t="s">
+    <row r="38" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F39" s="18" t="s">
+    <row r="39" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F39" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="20" t="s">
+    <row r="40" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F40" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -1068,8 +1242,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F41" s="21"/>
+    <row r="41" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F41" s="22"/>
       <c r="G41" s="3" t="s">
         <v>6</v>
       </c>
@@ -1079,31 +1253,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1111,25 +1285,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D5" s="9" t="s">
         <v>25</v>
       </c>
@@ -1149,14 +1323,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="4:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="18" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="12" t="s">
@@ -1169,7 +1343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
@@ -1189,7 +1363,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
@@ -1209,7 +1383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="4:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="17" t="s">
         <v>29</v>
       </c>
@@ -1230,6 +1404,126 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="42"/>
+      <c r="F11" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="42"/>
+      <c r="F12" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="45"/>
+      <c r="F13" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1465,18 +1759,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1499,14 +1793,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9672953C-5E67-45DC-94C9-EA4F7CDB7699}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1521,4 +1807,12 @@
     <ds:schemaRef ds:uri="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Use Case Definations for Assignment 2
</commit_message>
<xml_diff>
--- a/GroupD_RolesModel+InteractionModels.xlsx
+++ b/GroupD_RolesModel+InteractionModels.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\GroupD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srujan Patel\Desktop\SENG696_GroupD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A970AD78-2AE7-4013-8F3D-54D1D7336397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Schema" sheetId="1" r:id="rId1"/>
     <sheet name="Interaction Model" sheetId="2" r:id="rId2"/>
     <sheet name="Exceptions_ClientAgent" sheetId="3" r:id="rId3"/>
+    <sheet name="Exceptions_Appointment agent" sheetId="4" r:id="rId4"/>
+    <sheet name="Exceptions_NotificationAgent" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Role Schema</t>
   </si>
@@ -240,12 +243,51 @@
   </si>
   <si>
     <t>Client Information</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>Error Message is generated stating that no appointment slots are available</t>
+  </si>
+  <si>
+    <t>Clinic System Agent</t>
+  </si>
+  <si>
+    <t>Notification Agent, Clinic System Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System cannot book an appointment </t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>Error Message is generated stating that user is not reachable.</t>
+  </si>
+  <si>
+    <t>User not reachable at this point</t>
+  </si>
+  <si>
+    <t>Video Link Agent, Clinic System Agent</t>
+  </si>
+  <si>
+    <t>Data Required for Notification Agent</t>
+  </si>
+  <si>
+    <t>Video Link</t>
+  </si>
+  <si>
+    <t>Booked Appointment details</t>
+  </si>
+  <si>
+    <t>Email Address and Cell Phone Number of the user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -562,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -606,18 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -632,40 +662,55 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,11 +996,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F3:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,43 +1013,43 @@
   <sheetData>
     <row r="3" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1015,7 +1060,7 @@
       </c>
     </row>
     <row r="9" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="22"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1025,43 +1070,43 @@
     </row>
     <row r="11" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="20"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1072,7 +1117,7 @@
       </c>
     </row>
     <row r="17" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="22"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1082,43 +1127,43 @@
     </row>
     <row r="19" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="20"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="20"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1129,7 +1174,7 @@
       </c>
     </row>
     <row r="25" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="22"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="3" t="s">
         <v>6</v>
       </c>
@@ -1139,43 +1184,43 @@
     </row>
     <row r="27" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="20"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="20"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="20"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="20"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="5" t="s">
@@ -1186,7 +1231,7 @@
       </c>
     </row>
     <row r="33" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="22"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="3" t="s">
         <v>6</v>
       </c>
@@ -1196,43 +1241,43 @@
     </row>
     <row r="35" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G36" s="20"/>
+      <c r="G36" s="36"/>
       <c r="H36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="20"/>
+      <c r="G37" s="36"/>
       <c r="H37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="20"/>
+      <c r="G38" s="36"/>
       <c r="H38" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="20"/>
+      <c r="G39" s="36"/>
       <c r="H39" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="37" t="s">
         <v>4</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -1243,7 +1288,7 @@
       </c>
     </row>
     <row r="41" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F41" s="22"/>
+      <c r="F41" s="38"/>
       <c r="G41" s="3" t="s">
         <v>6</v>
       </c>
@@ -1253,31 +1298,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:F33"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1285,7 +1330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D4:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1410,11 +1455,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E3:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1426,91 +1471,91 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="23" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="42"/>
-      <c r="F11" s="43" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="42"/>
-      <c r="F12" s="43" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="45"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="46" t="s">
         <v>70</v>
       </c>
@@ -1529,7 +1574,273 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFA8A1D-D9ED-4F82-842B-DF283D549E15}">
+  <dimension ref="E1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E1:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="5:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="5:7" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="33"/>
+      <c r="F10" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="33"/>
+      <c r="F11" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="34"/>
+      <c r="F12" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5A35D9-4134-4641-95C2-5F99D8D4CDC4}">
+  <dimension ref="E1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="5:7" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="5:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="33"/>
+      <c r="F10" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="33"/>
+      <c r="F11" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="34"/>
+      <c r="F12" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100167A42814A0A7A429FBAAD58A3662C43" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e0f0b35447dfaef00fa2716150d7de8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8" xmlns:ns4="ce8d2f3a-208b-4f58-bb79-4192d7cf8650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b4fe6bd1d6509f7a3dbc01590a646f" ns3:_="" ns4:_="">
     <xsd:import namespace="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
@@ -1758,36 +2069,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E9EDBE-6CCD-4A05-942D-0FB6EAB02CCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
-    <ds:schemaRef ds:uri="ce8d2f3a-208b-4f58-bb79-4192d7cf8650"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1810,9 +2095,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E9EDBE-6CCD-4A05-942D-0FB6EAB02CCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
+    <ds:schemaRef ds:uri="ce8d2f3a-208b-4f58-bb79-4192d7cf8650"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Included Video Agent Invocation
</commit_message>
<xml_diff>
--- a/GroupD_RolesModel+InteractionModels.xlsx
+++ b/GroupD_RolesModel+InteractionModels.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srujan Patel\Desktop\SENG696_GroupD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\GroupD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A970AD78-2AE7-4013-8F3D-54D1D7336397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Role Schema" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
   <si>
     <t>Role Schema</t>
   </si>
@@ -83,9 +82,6 @@
   </si>
   <si>
     <t>Send MedicalReport to the User</t>
-  </si>
-  <si>
-    <t>GenerateReport</t>
   </si>
   <si>
     <t>createReport</t>
@@ -146,36 +142,18 @@
     <t>The service will listen to the appointment agent for a trigger. Once received, it will invoke the respective API to provide a meeting link to the user. Also, it will send a mail to the doctor to provide the patient feedback.</t>
   </si>
   <si>
-    <t>searchProfile</t>
-  </si>
-  <si>
     <t>Search in Database for user profile</t>
   </si>
   <si>
-    <t>SearchDatabase</t>
-  </si>
-  <si>
     <t>read Userprofile, write Database</t>
   </si>
   <si>
-    <t>newProfile = SearchDatabase.service</t>
-  </si>
-  <si>
-    <t>Successfully creating a profile</t>
-  </si>
-  <si>
     <t>createAppointment</t>
   </si>
   <si>
     <t>Creating new and successful appointment</t>
   </si>
   <si>
-    <t>createAppointment = createApppointment.service</t>
-  </si>
-  <si>
-    <t>Successfully generating an Appointment</t>
-  </si>
-  <si>
     <t>searchDatabase</t>
   </si>
   <si>
@@ -185,15 +163,9 @@
     <t>Clinic system</t>
   </si>
   <si>
-    <t>searchDatabse</t>
-  </si>
-  <si>
     <t xml:space="preserve">If any registered user visits portal, it will search the database for its previous logs and details and share it with the physician. </t>
   </si>
   <si>
-    <t xml:space="preserve">To create a new and repeated appointments with the doctor for the users  </t>
-  </si>
-  <si>
     <t>When a user wish to consult a physician, this service will generate appointments for the user with the physician. It will store the appointments in the database so that reminders can be sent.</t>
   </si>
   <si>
@@ -282,12 +254,72 @@
   </si>
   <si>
     <t>Email Address and Cell Phone Number of the user</t>
+  </si>
+  <si>
+    <t>searchAppointnment</t>
+  </si>
+  <si>
+    <t>deleteAppointnment</t>
+  </si>
+  <si>
+    <t>Delete Appointment previously scheduled by user</t>
+  </si>
+  <si>
+    <t>DeleteAppointment</t>
+  </si>
+  <si>
+    <t>read Userprofile, write Database, write UserProfile</t>
+  </si>
+  <si>
+    <t>newProfile = Appointment.Service</t>
+  </si>
+  <si>
+    <t>Successfully Delete an appointment</t>
+  </si>
+  <si>
+    <t>Successfully searching an existing appointment</t>
+  </si>
+  <si>
+    <t>Successfully generating a new Appointment</t>
+  </si>
+  <si>
+    <t>GeneratePdfReport</t>
+  </si>
+  <si>
+    <t>updateAppointnment</t>
+  </si>
+  <si>
+    <t>Update Appointment previously scheduled by user</t>
+  </si>
+  <si>
+    <t>UpdateAppointment</t>
+  </si>
+  <si>
+    <t>displayAppointnment</t>
+  </si>
+  <si>
+    <t>Showing Doctors/Clients the list of upcoming appointments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a new appointment with the doctor for the users  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a new appointments with the doctor for the users  </t>
+  </si>
+  <si>
+    <t>To Re-schedule the previously booked appointment</t>
+  </si>
+  <si>
+    <t>AppointmentService</t>
+  </si>
+  <si>
+    <t>Once the appointments are set, the user can choose another time between 9AM - 6PM to re-schedule the appointment. He will receive a mail from the clinic updating the details.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -600,11 +632,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -618,35 +689,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -670,6 +712,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,8 +754,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,11 +1092,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F3:H41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F3:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,320 +1105,459 @@
     <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="58.44140625" customWidth="1"/>
+    <col min="13" max="13" width="56.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="35" t="s">
+    <row r="3" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="36"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F6" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24"/>
+      <c r="L5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F7" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F8" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="6:12" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="38"/>
+        <v>80</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="26"/>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F12" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="6:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F13" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="36"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F14" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24"/>
+      <c r="L13" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="24"/>
+      <c r="L14" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="24"/>
+      <c r="L15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="38"/>
+      <c r="H16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="26"/>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="35" t="s">
+      <c r="J20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="24"/>
+      <c r="L20" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="35" t="s">
+      <c r="J21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="24"/>
+      <c r="L21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="36"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="35" t="s">
+      <c r="J22" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="24"/>
+      <c r="L22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F23" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="37" t="s">
+      <c r="J23" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="38"/>
+        <v>23</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="26"/>
       <c r="G25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F28" s="35" t="s">
+      <c r="J25" s="26"/>
+      <c r="K25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F29" s="35" t="s">
+      <c r="J28" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="24"/>
+      <c r="L28" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F30" s="35" t="s">
+      <c r="J29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="24"/>
+      <c r="L29" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="36"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F31" s="35" t="s">
+      <c r="J30" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="24"/>
+      <c r="L30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F31" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F32" s="37" t="s">
+      <c r="J31" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="24"/>
+      <c r="L31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="38"/>
+        <v>22</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="26"/>
       <c r="G33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F36" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F39" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="1" t="s">
+      <c r="J33" s="26"/>
+      <c r="K33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F41" s="38"/>
-      <c r="G41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="40">
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1330,122 +1565,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="D4:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1"/>
-    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="9" t="s">
+    <row r="4" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E6" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="200.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="F9" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="J9" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="53" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1455,11 +1722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E3:G13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,95 +1738,95 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="22" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="F10" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="19" t="s">
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="20"/>
+      <c r="F11" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="26" t="s">
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="20"/>
+      <c r="F12" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="21"/>
+      <c r="F13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="40"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="29"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="33"/>
-      <c r="F11" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="33"/>
-      <c r="F12" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="45"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="34"/>
-      <c r="F13" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="47"/>
+      <c r="G13" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1575,11 +1842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFA8A1D-D9ED-4F82-842B-DF283D549E15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E1:G12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,102 +1857,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="5:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="5:7" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="5:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="22" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="F9" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="5:7" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="19" t="s">
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="20"/>
+      <c r="F10" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="26" t="s">
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="20"/>
+      <c r="F11" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="33"/>
-      <c r="F10" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="33"/>
-      <c r="F11" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="45"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="34"/>
-      <c r="F12" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="47"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1700,10 +1967,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5A35D9-4134-4641-95C2-5F99D8D4CDC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1715,102 +1982,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="5:7" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="5:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="5:7" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="22" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="5:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="39" t="s">
+      <c r="F9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="20"/>
+      <c r="F10" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="20"/>
+      <c r="F11" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="21"/>
+      <c r="F12" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="33"/>
-      <c r="F10" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="33"/>
-      <c r="F11" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="34"/>
-      <c r="F12" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="47"/>
+      <c r="G12" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1826,21 +2093,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100167A42814A0A7A429FBAAD58A3662C43" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e0f0b35447dfaef00fa2716150d7de8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8" xmlns:ns4="ce8d2f3a-208b-4f58-bb79-4192d7cf8650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b4fe6bd1d6509f7a3dbc01590a646f" ns3:_="" ns4:_="">
     <xsd:import namespace="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
@@ -2069,10 +2321,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E9EDBE-6CCD-4A05-942D-0FB6EAB02CCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
+    <ds:schemaRef ds:uri="ce8d2f3a-208b-4f58-bb79-4192d7cf8650"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2095,20 +2373,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E9EDBE-6CCD-4A05-942D-0FB6EAB02CCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749B839-709D-4D5F-A95C-E1648B2B3F05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8a3f0a0-49e1-415f-8d7d-9b51d0eb93e8"/>
-    <ds:schemaRef ds:uri="ce8d2f3a-208b-4f58-bb79-4192d7cf8650"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>